<commit_message>
Commentaire répartition taches dans code arduino
</commit_message>
<xml_diff>
--- a/Taches a effectuer.xlsx
+++ b/Taches a effectuer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soufian\Desktop\INSA\2018\MOSH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DA43DB-EA9E-47B1-967F-73EAEC664082}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E4763F-E55B-47B8-9EDF-E077AB29E72E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24980" windowHeight="10160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -238,10 +238,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -540,22 +540,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -569,7 +569,7 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <v>43115</v>
       </c>
     </row>
@@ -580,12 +580,12 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -778,7 +778,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C21" s="8">
         <v>5</v>

</xml_diff>

<commit_message>
Inversion roles quentin/souf dans le code
</commit_message>
<xml_diff>
--- a/Taches a effectuer.xlsx
+++ b/Taches a effectuer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soufian\Desktop\INSA\2018\MOSH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E4763F-E55B-47B8-9EDF-E077AB29E72E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05A1176-22CC-4BF0-8F8D-CA6966D51A60}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24980" windowHeight="10160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,7 +525,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -857,7 +857,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>31</v>
@@ -891,7 +891,7 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Ajout de liste des dimensions - MAJ des taches
</commit_message>
<xml_diff>
--- a/Taches a effectuer.xlsx
+++ b/Taches a effectuer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soufian\Desktop\INSA\2018\MOSH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05A1176-22CC-4BF0-8F8D-CA6966D51A60}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522861DA-27AC-4DD6-A7D7-12326BDDCAA9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24980" windowHeight="10160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="38">
   <si>
     <t>Nicolas</t>
   </si>
@@ -525,7 +525,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -746,7 +746,7 @@
       <c r="B19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>3</v>
       </c>
       <c r="D19" s="1"/>
@@ -859,11 +859,11 @@
       <c r="B26" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
       <c r="F26" s="1"/>
       <c r="G26" s="11">
         <v>3</v>
@@ -893,7 +893,7 @@
       <c r="B28" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D28" s="1"/>

</xml_diff>

<commit_message>
PCB corrigé et verifié. Typon prêt
</commit_message>
<xml_diff>
--- a/Taches a effectuer.xlsx
+++ b/Taches a effectuer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soufian\Desktop\INSA\2018\MOSH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522861DA-27AC-4DD6-A7D7-12326BDDCAA9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF257EB7-03A4-429C-B07F-D48D9E74A514}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24980" windowHeight="10160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,7 +525,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -688,8 +688,8 @@
         <v>30</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
       <c r="G15" s="11">
         <v>3</v>
       </c>
@@ -749,7 +749,7 @@
       <c r="C19" s="7">
         <v>3</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="11">

</xml_diff>

<commit_message>
Correction comportement erratique moteurs + Fonction US et LUX pris en compte + Tests en environnement hostile
</commit_message>
<xml_diff>
--- a/Taches a effectuer.xlsx
+++ b/Taches a effectuer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soufian\Desktop\INSA\2018\MOSH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6086EB22-939A-4D72-B7B7-13AED4625829}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C53E77D-29B4-4134-9288-F22622486A20}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24980" windowHeight="10160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,9 +286,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -301,6 +298,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,7 +584,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -599,22 +599,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -639,12 +639,12 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -754,27 +754,27 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="20">
         <v>3</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23" t="s">
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="8">
@@ -826,9 +826,9 @@
         <v>3</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="11">
+      <c r="E20" s="23"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="12">
         <v>4</v>
       </c>
     </row>
@@ -837,7 +837,7 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="8">
         <v>4</v>
@@ -867,11 +867,11 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="20" t="s">
-        <v>1</v>
+      <c r="B23" s="19" t="s">
+        <v>0</v>
       </c>
       <c r="C23" s="8">
         <v>3</v>
@@ -884,10 +884,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -933,7 +933,7 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C27" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
Mise a jour des taches effectuees
</commit_message>
<xml_diff>
--- a/Taches a effectuer.xlsx
+++ b/Taches a effectuer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soufian\Desktop\INSA\2018\MOSH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C53E77D-29B4-4134-9288-F22622486A20}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398F62F4-B433-401E-A650-4A746E9091BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24980" windowHeight="10160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="40">
   <si>
     <t>Nicolas</t>
   </si>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -669,7 +669,7 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="11" t="s">
         <v>33</v>
       </c>
@@ -777,13 +777,13 @@
       <c r="B17" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>3</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="11" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="12" t="s">
         <v>32</v>
       </c>
     </row>
@@ -839,13 +839,13 @@
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>4</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="11">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="12">
         <v>5</v>
       </c>
     </row>
@@ -856,13 +856,13 @@
       <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>5</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="11" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="12" t="s">
         <v>35</v>
       </c>
     </row>
@@ -873,13 +873,13 @@
       <c r="B23" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>3</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="11" t="s">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="12" t="s">
         <v>32</v>
       </c>
     </row>
@@ -907,12 +907,12 @@
       <c r="B25" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
       <c r="G25" s="11">
         <v>7</v>
       </c>
@@ -938,10 +938,10 @@
       <c r="C27" s="7">
         <v>1</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="11" t="s">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -958,7 +958,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="11">
+      <c r="G28" s="12">
         <v>3</v>
       </c>
     </row>
@@ -969,13 +969,13 @@
       <c r="B29" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="11">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="12">
         <v>3</v>
       </c>
     </row>
@@ -990,9 +990,9 @@
         <v>31</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="11">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="12">
         <v>3</v>
       </c>
     </row>

</xml_diff>